<commit_message>
Login Test Cases Addd
</commit_message>
<xml_diff>
--- a/Demo_Website_Testing/Test_Case_Design/Login_Test_Cases.xlsx
+++ b/Demo_Website_Testing/Test_Case_Design/Login_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wasana\University\Projects\QA-Portfolio\Demo_Website_Testing\Test_Case_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FFAEA1-4908-4BAC-B8C4-6A0FD5E0C8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769606A5-0953-4FF1-9C0A-17C2F5786982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
   <si>
     <t>Test Case Title</t>
   </si>
@@ -58,13 +58,302 @@
   </si>
   <si>
     <t>Test Scenario ID</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-01</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-02</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-03</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-04</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-05</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-06</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-07</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-08</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-09</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-10</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-11</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-12</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-01</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-02</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-03</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-04</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-05</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-06</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-07</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-08</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-09</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-10</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-11</t>
+  </si>
+  <si>
+    <t>TS-LOGIN-12</t>
+  </si>
+  <si>
+    <t>Verify login with invalid email</t>
+  </si>
+  <si>
+    <t>Verify login with valid email and password</t>
+  </si>
+  <si>
+    <t>Verify login with invalid password</t>
+  </si>
+  <si>
+    <t>Verify login with empty email and password</t>
+  </si>
+  <si>
+    <t>Verify login with empty email field</t>
+  </si>
+  <si>
+    <t>Verify login with empty password field</t>
+  </si>
+  <si>
+    <t>Verify error message for invalid login</t>
+  </si>
+  <si>
+    <t>Verify successful navigation after login</t>
+  </si>
+  <si>
+    <t>Verify logout functionality</t>
+  </si>
+  <si>
+    <t>Verify session handling after logout</t>
+  </si>
+  <si>
+    <t>Verify login on different browsers</t>
+  </si>
+  <si>
+    <t>Verify login on mobile devices</t>
+  </si>
+  <si>
+    <t>User is registered
+Login page is open</t>
+  </si>
+  <si>
+    <t>Login page is open</t>
+  </si>
+  <si>
+    <t>User is registered</t>
+  </si>
+  <si>
+    <t>User is logged in</t>
+  </si>
+  <si>
+    <t>User logged out</t>
+  </si>
+  <si>
+    <t>Browsers installed</t>
+  </si>
+  <si>
+    <t>Mobile device or responsive mode</t>
+  </si>
+  <si>
+    <t>1. Enter valid email
+2.Enter valid password
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>1. Enter invalid email
+2.Enter valid password
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>1. Enter valid email
+2.Enter invalid password
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>1. Leave email field empty
+2. Leave password field empty
+3. Click Login</t>
+  </si>
+  <si>
+    <t>1. Enter valid email
+2. Leave password empty
+3. Click Login</t>
+  </si>
+  <si>
+    <t>1. Enter invalid credentials
+2. Click Login</t>
+  </si>
+  <si>
+    <t>1. Enter valid credentials
+2. Click Login</t>
+  </si>
+  <si>
+    <t>1. Click Logout button</t>
+  </si>
+  <si>
+    <t>1. Click browser Back button
+2. Try accessing dashboard URL</t>
+  </si>
+  <si>
+    <t>1. Open site in Chrome, Firefox, Edge
+2. Perform login</t>
+  </si>
+  <si>
+    <t>1. Open site on mobile
+2. Enter valid credentials
+3. Click Login</t>
+  </si>
+  <si>
+    <t>Email: nimali@gmail.com
+Password: nimali12345</t>
+  </si>
+  <si>
+    <t>Email: nimal@gmail.com
+Password: nimali12346</t>
+  </si>
+  <si>
+    <t>Email: nimali@gmail.com
+Password: nimali1234</t>
+  </si>
+  <si>
+    <t>N / A</t>
+  </si>
+  <si>
+    <t>1. Leave email field empty
+2. Enter valid password
+3. Click Login</t>
+  </si>
+  <si>
+    <t>Email: 
+Password: nimali12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: nimali@gmail.com
+Password: </t>
+  </si>
+  <si>
+    <t>Email: nimal@gmail.com
+Password: nimali1234</t>
+  </si>
+  <si>
+    <t>User should be logged in successfully and redirected to Home page</t>
+  </si>
+  <si>
+    <t>Error message should be displayed</t>
+  </si>
+  <si>
+    <t>Validation messages should be displayed</t>
+  </si>
+  <si>
+    <t>Email validation message should be displayed</t>
+  </si>
+  <si>
+    <t>Password validation message should be displayed</t>
+  </si>
+  <si>
+    <t>Error message should be clear and user-friendly</t>
+  </si>
+  <si>
+    <t>User should be redirected to Home page</t>
+  </si>
+  <si>
+    <t>User should be logged out successfully</t>
+  </si>
+  <si>
+    <t>User should not access protected pages</t>
+  </si>
+  <si>
+    <t>Login should work on all browsers</t>
+  </si>
+  <si>
+    <t>Login should work correctly on mobile</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>User  logged in successfully and redirected to Home page</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Error message displayed</t>
+  </si>
+  <si>
+    <t>Validation messages  displayed</t>
+  </si>
+  <si>
+    <t>Email validation message displayed</t>
+  </si>
+  <si>
+    <t>Password validation message displayed</t>
+  </si>
+  <si>
+    <t>Error message clear and user-friendly</t>
+  </si>
+  <si>
+    <t>User redirected to Home page</t>
+  </si>
+  <si>
+    <t>User  logged out successfully</t>
+  </si>
+  <si>
+    <t>User accessed protected pages</t>
+  </si>
+  <si>
+    <t>Login worked on all browsers</t>
+  </si>
+  <si>
+    <t>Login worked correctly on mobile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +369,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -89,7 +384,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -112,14 +407,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -401,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,47 +730,444 @@
     <col min="4" max="4" width="33.6640625" customWidth="1"/>
     <col min="5" max="5" width="35.21875" customWidth="1"/>
     <col min="6" max="6" width="45.21875" customWidth="1"/>
-    <col min="7" max="7" width="40.33203125" customWidth="1"/>
-    <col min="8" max="8" width="45" customWidth="1"/>
-    <col min="9" max="9" width="66.88671875" customWidth="1"/>
+    <col min="7" max="7" width="57.44140625" customWidth="1"/>
+    <col min="8" max="8" width="47.88671875" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>